<commit_message>
chap me bat ngo
</commit_message>
<xml_diff>
--- a/LuaChonCapTien.xlsx
+++ b/LuaChonCapTien.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Người thực hiện:</t>
   </si>
@@ -160,6 +160,21 @@
   </si>
   <si>
     <t>Ít nhất là trên khung H1 hay H4 để đảm bảo cho việc giao dịch ngắn hạn trong ngày hoặc trong tuần</t>
+  </si>
+  <si>
+    <t>Phản ứng rõ ràng khi tiếp xúc với keylevel</t>
+  </si>
+  <si>
+    <t>Hình thành những keylevel rõ ràng</t>
+  </si>
+  <si>
+    <t>Chúng ta cần tìm những cặp tiền chạy rõ ràng, dứt khoát</t>
+  </si>
+  <si>
+    <t>Nhiều cặp tiền nó chạy nhây một cách khó tả</t>
+  </si>
+  <si>
+    <t>Và hình thành những cây nến toàn râu là râu, việc này dẫn đến khó phân tích và khi vào lệnh dễ dính stoploss</t>
   </si>
 </sst>
 </file>
@@ -538,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,6 +941,32 @@
       <c r="B68">
         <v>5</v>
       </c>
+      <c r="C68" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>6</v>
+      </c>
+      <c r="C70" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>